<commit_message>
Final files for submission
</commit_message>
<xml_diff>
--- a/Kaggle/images/Graphiques.xlsx
+++ b/Kaggle/images/Graphiques.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume\Documents\~Coding\Python\INF8245E\Kaggle\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEEEFF4-DB1C-41D8-90EF-7C8026F5EAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E961E0-27E4-4DDE-8A2E-3DBF30C45823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3D33614-3FBD-47B8-8D97-9C78A990371D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Effect of fine-tuning" sheetId="1" r:id="rId1"/>
+    <sheet name="Effect of HP" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Before</t>
   </si>
@@ -51,9 +52,6 @@
     <t>DeeperVGG</t>
   </si>
   <si>
-    <t>DeeperVGG2</t>
-  </si>
-  <si>
     <t>VGG+Res</t>
   </si>
   <si>
@@ -61,6 +59,27 @@
   </si>
   <si>
     <t>SimpleNet</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>WideResNet 1</t>
+  </si>
+  <si>
+    <t>Dropout</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>Directly</t>
   </si>
 </sst>
 </file>
@@ -103,9 +122,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,9 +187,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$6:$F$11</c:f>
+              <c:f>'Effect of fine-tuning'!$F$6:$F$10</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>VGG</c:v>
                 </c:pt>
@@ -174,15 +197,12 @@
                   <c:v>DeeperVGG</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>DeeperVGG2</c:v>
+                  <c:v>VGG+Res</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VGG+Res</c:v>
+                  <c:v>WideResNet</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>WideResNet</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>SimpleNet</c:v>
                 </c:pt>
               </c:strCache>
@@ -190,10 +210,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$6:$G$11</c:f>
+              <c:f>'Effect of fine-tuning'!$G$6:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>69</c:v>
                 </c:pt>
@@ -201,15 +221,12 @@
                   <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>79</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>70</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>82</c:v>
                 </c:pt>
               </c:numCache>
@@ -241,9 +258,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$6:$F$11</c:f>
+              <c:f>'Effect of fine-tuning'!$F$6:$F$10</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>VGG</c:v>
                 </c:pt>
@@ -251,15 +268,12 @@
                   <c:v>DeeperVGG</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>DeeperVGG2</c:v>
+                  <c:v>VGG+Res</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>VGG+Res</c:v>
+                  <c:v>WideResNet</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>WideResNet</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>SimpleNet</c:v>
                 </c:pt>
               </c:strCache>
@@ -267,10 +281,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$6:$H$11</c:f>
+              <c:f>'Effect of fine-tuning'!$H$6:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>80</c:v>
                 </c:pt>
@@ -278,15 +292,12 @@
                   <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>84</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>79</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>89</c:v>
                 </c:pt>
               </c:numCache>
@@ -366,6 +377,8 @@
         <c:axId val="624619328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="90"/>
+          <c:min val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -555,9 +568,1735 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Effect of HP'!$C$6:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Effect of HP'!$D$6:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6D62-4FD2-AA30-7DBF0B215A35}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>In final model</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Effect of HP'!$C$8,'Effect of HP'!$C$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Effect of HP'!$E$8,'Effect of HP'!$E$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6D62-4FD2-AA30-7DBF0B215A35}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="64002320"/>
+        <c:axId val="64003152"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64002320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Dropout</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64003152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64003152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>F1 Score (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64002320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+          <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Effect of HP'!$C$15:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Effect of HP'!$D$15:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-90DC-4DC5-862E-E701F273B9CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>In final model</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Effect of HP'!$C$16:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Effect of HP'!$D$16:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-90DC-4DC5-862E-E701F273B9CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="64002320"/>
+        <c:axId val="64003152"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64002320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Dropout</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64003152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64003152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>F1 Score (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64002320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+          <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-5208-4B3E-9C22-9EF3503F2696}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-5208-4B3E-9C22-9EF3503F2696}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-5208-4B3E-9C22-9EF3503F2696}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Effect of HP'!$C$26:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0000000000000004E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.9999999999999994E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9999999999999999E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Effect of HP'!$D$26:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5208-4B3E-9C22-9EF3503F2696}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="64002320"/>
+        <c:axId val="64003152"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent5">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dPt>
+                  <c:idx val="0"/>
+                  <c:marker>
+                    <c:symbol val="circle"/>
+                    <c:size val="5"/>
+                    <c:spPr>
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:ln w="9525">
+                        <a:noFill/>
+                      </a:ln>
+                      <a:effectLst/>
+                    </c:spPr>
+                  </c:marker>
+                  <c:bubble3D val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000006-5208-4B3E-9C22-9EF3503F2696}"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="1"/>
+                  <c:marker>
+                    <c:symbol val="circle"/>
+                    <c:size val="5"/>
+                    <c:spPr>
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:ln w="9525">
+                        <a:noFill/>
+                      </a:ln>
+                      <a:effectLst/>
+                    </c:spPr>
+                  </c:marker>
+                  <c:bubble3D val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000004-5208-4B3E-9C22-9EF3503F2696}"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="2"/>
+                  <c:marker>
+                    <c:symbol val="circle"/>
+                    <c:size val="5"/>
+                    <c:spPr>
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:ln w="9525">
+                        <a:noFill/>
+                      </a:ln>
+                      <a:effectLst/>
+                    </c:spPr>
+                  </c:marker>
+                  <c:bubble3D val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000005-5208-4B3E-9C22-9EF3503F2696}"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dPt>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Effect of HP'!$C$27:$C$29</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00E+00</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>5.0000000000000001E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2.0000000000000001E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>4.0000000000000003E-5</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Effect of HP'!$D$27:$D$29</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="0">
+                        <c:v>89</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>88</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>87</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-5208-4B3E-9C22-9EF3503F2696}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64002320"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="5.000000000000001E-3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>L2</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64003152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64003152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>F1 Score (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64002320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+          <a:ea typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="25">
   <a:schemeClr val="accent5"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -1045,6 +2784,1554 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1070,14 +4357,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>455544</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>49695</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>185736</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1097,6 +4384,123 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F27B7901-8F7C-431C-9A9C-FA8608CDBD1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CF946ED-95D8-410C-8C5B-8ACE87D4B2E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C9A439E-0C24-4BDE-92F3-BC5A993624ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1402,10 +4806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29611D03-9507-4CE1-B9F5-3591C0A5AE86}">
-  <dimension ref="F5:V11"/>
+  <dimension ref="F5:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,10 +4856,10 @@
         <v>5</v>
       </c>
       <c r="G8">
+        <v>70</v>
+      </c>
+      <c r="H8">
         <v>79</v>
-      </c>
-      <c r="H8">
-        <v>84</v>
       </c>
     </row>
     <row r="9" spans="6:22" x14ac:dyDescent="0.25">
@@ -1463,10 +4867,10 @@
         <v>6</v>
       </c>
       <c r="G9">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="H9">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="6:22" x14ac:dyDescent="0.25">
@@ -1474,20 +4878,9 @@
         <v>7</v>
       </c>
       <c r="G10">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H10">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11">
-        <v>82</v>
-      </c>
-      <c r="H11">
         <v>89</v>
       </c>
     </row>
@@ -1496,4 +4889,288 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F97F76-580F-450F-B645-782BC9831682}">
+  <dimension ref="B4:E35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>0.4</v>
+      </c>
+      <c r="D6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7">
+        <v>0.3</v>
+      </c>
+      <c r="D7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>84</v>
+      </c>
+      <c r="E8">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0.6</v>
+      </c>
+      <c r="D9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0.3</v>
+      </c>
+      <c r="D10">
+        <v>83</v>
+      </c>
+      <c r="E10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0.6</v>
+      </c>
+      <c r="D11">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16">
+        <v>0.2</v>
+      </c>
+      <c r="D16">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17">
+        <v>0.1</v>
+      </c>
+      <c r="D17">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>0.1</v>
+      </c>
+      <c r="D18">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>0.2</v>
+      </c>
+      <c r="D20">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>0.4</v>
+      </c>
+      <c r="D21">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="D26">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D27">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="D28">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="D29">
+        <v>87</v>
+      </c>
+      <c r="E29">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="D30">
+        <v>87</v>
+      </c>
+      <c r="E30">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="D31">
+        <v>86</v>
+      </c>
+      <c r="E31">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="D32">
+        <v>86</v>
+      </c>
+      <c r="E32">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="D33">
+        <v>85</v>
+      </c>
+      <c r="E33">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D34">
+        <v>85</v>
+      </c>
+      <c r="E34">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B26:B28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>